<commit_message>
main.js and elm talk
</commit_message>
<xml_diff>
--- a/notes/conditions.xlsx
+++ b/notes/conditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/momo/Dropbox/projects/connectives-qud/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDAF556-6CB1-DE42-AC3E-0DBCA9FB7AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AB6CEB-78E8-C240-B9D2-13D423CE7D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37840" yWindow="1300" windowWidth="23720" windowHeight="20240" activeTab="5" xr2:uid="{3AB9929D-0A0B-1747-A8A7-16F45675C35B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20240" xr2:uid="{3AB9929D-0A0B-1747-A8A7-16F45675C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="overall" sheetId="9" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2420" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2408" uniqueCount="356">
   <si>
     <t>QUD</t>
   </si>
@@ -1337,7 +1337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1451,6 +1451,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1777,15 +1784,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD98CBC-AE24-7441-ABC5-9741245297FD}">
   <dimension ref="A1:N142"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="114" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="163" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="31" customWidth="1"/>
     <col min="6" max="6" width="22.1640625" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
     <col min="8" max="8" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2720,7 +2727,7 @@
         <v>19</v>
       </c>
       <c r="C30" s="26"/>
-      <c r="D30" s="26" t="s">
+      <c r="D30" s="30" t="s">
         <v>233</v>
       </c>
       <c r="E30" s="26" t="s">
@@ -2772,7 +2779,7 @@
       <c r="B32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="26" t="s">
+      <c r="D32" s="30" t="s">
         <v>234</v>
       </c>
       <c r="E32" s="26" t="s">
@@ -2824,7 +2831,7 @@
       <c r="B34" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="26" t="s">
+      <c r="D34" s="30" t="s">
         <v>236</v>
       </c>
       <c r="E34" s="26" t="s">
@@ -2876,7 +2883,7 @@
       <c r="B36" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="26" t="s">
+      <c r="D36" s="30" t="s">
         <v>238</v>
       </c>
       <c r="E36" s="26" t="s">
@@ -2922,25 +2929,27 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
+      <c r="A38" s="94">
         <v>9</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="D38" s="26" t="s">
+      <c r="C38" s="94"/>
+      <c r="D38" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E38" s="26" t="s">
+      <c r="E38" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F38" s="94" t="s">
         <v>151</v>
       </c>
-      <c r="G38" s="26" t="s">
+      <c r="G38" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="H38" s="94"/>
+      <c r="I38" s="94" t="s">
         <v>14</v>
       </c>
       <c r="K38" s="26" t="s">
@@ -2948,25 +2957,27 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
+      <c r="A39" s="94">
         <v>10</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="D39" s="26" t="s">
+      <c r="C39" s="94"/>
+      <c r="D39" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E39" s="26" t="s">
+      <c r="E39" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" s="94" t="s">
         <v>153</v>
       </c>
-      <c r="G39" s="26" t="s">
+      <c r="G39" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="H39" s="94"/>
+      <c r="I39" s="94" t="s">
         <v>14</v>
       </c>
       <c r="K39" s="26" t="s">
@@ -2974,25 +2985,27 @@
       </c>
     </row>
     <row r="40" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
+      <c r="A40" s="94">
         <v>11</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="C40" s="94"/>
+      <c r="D40" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="E40" s="26" t="s">
+      <c r="E40" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" s="94" t="s">
         <v>151</v>
       </c>
-      <c r="G40" s="26" t="s">
+      <c r="G40" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="H40" s="94"/>
+      <c r="I40" s="94" t="s">
         <v>14</v>
       </c>
       <c r="K40" s="26" t="s">
@@ -3000,25 +3013,27 @@
       </c>
     </row>
     <row r="41" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+      <c r="A41" s="94">
         <v>12</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="C41" s="94"/>
+      <c r="D41" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="E41" s="26" t="s">
+      <c r="E41" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F41" s="94" t="s">
         <v>153</v>
       </c>
-      <c r="G41" s="26" t="s">
+      <c r="G41" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="H41" s="94"/>
+      <c r="I41" s="94" t="s">
         <v>14</v>
       </c>
       <c r="K41" s="26" t="s">
@@ -3035,24 +3050,20 @@
       <c r="C42" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="D42" s="85" t="s">
-        <v>144</v>
+      <c r="D42" s="35" t="s">
+        <v>285</v>
       </c>
       <c r="E42" s="86"/>
-      <c r="F42" s="35" t="s">
-        <v>285</v>
-      </c>
-      <c r="G42" s="86"/>
+      <c r="F42" s="86" t="s">
+        <v>153</v>
+      </c>
+      <c r="G42" s="86" t="s">
+        <v>341</v>
+      </c>
       <c r="H42" s="86" t="s">
-        <v>153</v>
-      </c>
-      <c r="I42" s="86" t="s">
-        <v>341</v>
-      </c>
-      <c r="J42" s="86" t="s">
         <v>340</v>
       </c>
-      <c r="K42" s="36" t="s">
+      <c r="I42" s="36" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3066,24 +3077,20 @@
       <c r="C43" s="87" t="s">
         <v>144</v>
       </c>
-      <c r="D43" s="87" t="s">
-        <v>145</v>
+      <c r="D43" s="26" t="s">
+        <v>290</v>
       </c>
       <c r="E43" s="46"/>
       <c r="F43" s="26" t="s">
-        <v>290</v>
-      </c>
-      <c r="G43" s="46"/>
+        <v>153</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>344</v>
+      </c>
       <c r="H43" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="I43" s="26" t="s">
-        <v>344</v>
-      </c>
-      <c r="J43" s="26" t="s">
         <v>340</v>
       </c>
-      <c r="K43" s="33" t="s">
+      <c r="I43" s="33" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3097,24 +3104,20 @@
       <c r="C44" s="87" t="s">
         <v>145</v>
       </c>
-      <c r="D44" s="87" t="s">
-        <v>144</v>
+      <c r="D44" s="26" t="s">
+        <v>343</v>
       </c>
       <c r="E44" s="46"/>
       <c r="F44" s="26" t="s">
-        <v>343</v>
-      </c>
-      <c r="G44" s="46"/>
+        <v>151</v>
+      </c>
+      <c r="G44" s="26" t="s">
+        <v>342</v>
+      </c>
       <c r="H44" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="I44" s="26" t="s">
-        <v>342</v>
-      </c>
-      <c r="J44" s="26" t="s">
         <v>346</v>
       </c>
-      <c r="K44" s="33" t="s">
+      <c r="I44" s="33" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3128,24 +3131,20 @@
       <c r="C45" s="87" t="s">
         <v>144</v>
       </c>
-      <c r="D45" s="87" t="s">
-        <v>145</v>
-      </c>
-      <c r="E45" s="26"/>
+      <c r="D45" s="26" t="s">
+        <v>345</v>
+      </c>
+      <c r="E45" s="46"/>
       <c r="F45" s="26" t="s">
-        <v>345</v>
-      </c>
-      <c r="G45" s="46"/>
+        <v>151</v>
+      </c>
+      <c r="G45" s="26" t="s">
+        <v>106</v>
+      </c>
       <c r="H45" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="I45" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="J45" s="26" t="s">
         <v>346</v>
       </c>
-      <c r="K45" s="33" t="s">
+      <c r="I45" s="33" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3159,24 +3158,20 @@
       <c r="C46" s="87" t="s">
         <v>145</v>
       </c>
-      <c r="D46" s="87" t="s">
-        <v>144</v>
-      </c>
-      <c r="E46" s="26"/>
+      <c r="D46" s="26" t="s">
+        <v>347</v>
+      </c>
+      <c r="E46" s="46"/>
       <c r="F46" s="26" t="s">
-        <v>347</v>
-      </c>
-      <c r="G46" s="46"/>
+        <v>101</v>
+      </c>
+      <c r="G46" s="26" t="s">
+        <v>117</v>
+      </c>
       <c r="H46" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="I46" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="J46" s="26" t="s">
         <v>338</v>
       </c>
-      <c r="K46" s="33" t="s">
+      <c r="I46" s="33" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3190,24 +3185,20 @@
       <c r="C47" s="88" t="s">
         <v>144</v>
       </c>
-      <c r="D47" s="88" t="s">
-        <v>145</v>
-      </c>
-      <c r="E47" s="38"/>
+      <c r="D47" s="89" t="s">
+        <v>170</v>
+      </c>
+      <c r="E47" s="89"/>
       <c r="F47" s="89" t="s">
-        <v>170</v>
-      </c>
-      <c r="G47" s="89"/>
+        <v>348</v>
+      </c>
+      <c r="G47" s="89" t="s">
+        <v>349</v>
+      </c>
       <c r="H47" s="89" t="s">
-        <v>348</v>
-      </c>
-      <c r="I47" s="89" t="s">
-        <v>349</v>
-      </c>
-      <c r="J47" s="89" t="s">
         <v>338</v>
       </c>
-      <c r="K47" s="33" t="s">
+      <c r="I47" s="33" t="s">
         <v>14</v>
       </c>
       <c r="M47" t="s">
@@ -3215,64 +3206,56 @@
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
+      <c r="A48" s="94">
         <v>19</v>
       </c>
-      <c r="B48" s="83" t="s">
+      <c r="B48" s="95" t="s">
         <v>299</v>
       </c>
-      <c r="C48" s="87" t="s">
-        <v>145</v>
-      </c>
-      <c r="D48" s="87" t="s">
-        <v>144</v>
-      </c>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26" t="s">
+      <c r="C48" s="96" t="s">
+        <v>145</v>
+      </c>
+      <c r="D48" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="G48" s="46"/>
-      <c r="H48" s="26" t="s">
+      <c r="E48" s="30"/>
+      <c r="F48" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="I48" s="26" t="s">
+      <c r="G48" s="30" t="s">
         <v>329</v>
       </c>
-      <c r="J48" s="26" t="s">
+      <c r="H48" s="30" t="s">
         <v>339</v>
       </c>
-      <c r="K48" s="33" t="s">
+      <c r="I48" s="97" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
+      <c r="A49" s="94">
         <v>20</v>
       </c>
-      <c r="B49" s="83" t="s">
+      <c r="B49" s="95" t="s">
         <v>300</v>
       </c>
-      <c r="C49" s="87" t="s">
-        <v>144</v>
-      </c>
-      <c r="D49" s="87" t="s">
-        <v>145</v>
-      </c>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26" t="s">
+      <c r="C49" s="96" t="s">
+        <v>144</v>
+      </c>
+      <c r="D49" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="G49" s="46"/>
-      <c r="H49" s="26" t="s">
+      <c r="E49" s="30"/>
+      <c r="F49" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="I49" s="26" t="s">
+      <c r="G49" s="30" t="s">
         <v>350</v>
       </c>
-      <c r="J49" s="26" t="s">
+      <c r="H49" s="30" t="s">
         <v>339</v>
       </c>
-      <c r="K49" s="33" t="s">
+      <c r="I49" s="97" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3286,24 +3269,20 @@
       <c r="C50" s="87" t="s">
         <v>145</v>
       </c>
-      <c r="D50" s="87" t="s">
-        <v>144</v>
-      </c>
-      <c r="E50" s="26"/>
+      <c r="D50" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="E50" s="46"/>
       <c r="F50" s="26" t="s">
-        <v>351</v>
-      </c>
-      <c r="G50" s="46"/>
+        <v>151</v>
+      </c>
+      <c r="G50" s="26" t="s">
+        <v>62</v>
+      </c>
       <c r="H50" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="I50" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="J50" s="26" t="s">
         <v>339</v>
       </c>
-      <c r="K50" s="33" t="s">
+      <c r="I50" s="33" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3317,24 +3296,20 @@
       <c r="C51" s="87" t="s">
         <v>144</v>
       </c>
-      <c r="D51" s="87" t="s">
-        <v>145</v>
-      </c>
-      <c r="E51" s="26"/>
+      <c r="D51" s="26" t="s">
+        <v>321</v>
+      </c>
+      <c r="E51" s="46"/>
       <c r="F51" s="26" t="s">
-        <v>321</v>
-      </c>
-      <c r="G51" s="46"/>
+        <v>151</v>
+      </c>
+      <c r="G51" s="26" t="s">
+        <v>352</v>
+      </c>
       <c r="H51" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="I51" s="26" t="s">
-        <v>352</v>
-      </c>
-      <c r="J51" s="26" t="s">
         <v>339</v>
       </c>
-      <c r="K51" s="33" t="s">
+      <c r="I51" s="33" t="s">
         <v>14</v>
       </c>
       <c r="M51" t="s">
@@ -3351,24 +3326,20 @@
       <c r="C52" s="87" t="s">
         <v>145</v>
       </c>
-      <c r="D52" s="87" t="s">
-        <v>144</v>
-      </c>
-      <c r="E52" s="26"/>
-      <c r="F52" s="52" t="s">
+      <c r="D52" s="52" t="s">
         <v>355</v>
       </c>
-      <c r="G52" s="46"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="26" t="s">
+        <v>353</v>
+      </c>
+      <c r="G52" s="26" t="s">
+        <v>281</v>
+      </c>
       <c r="H52" s="26" t="s">
-        <v>353</v>
-      </c>
-      <c r="I52" s="26" t="s">
-        <v>281</v>
-      </c>
-      <c r="J52" s="26" t="s">
         <v>339</v>
       </c>
-      <c r="K52" s="33" t="s">
+      <c r="I52" s="33" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3382,24 +3353,20 @@
       <c r="C53" s="88" t="s">
         <v>144</v>
       </c>
-      <c r="D53" s="88" t="s">
-        <v>145</v>
+      <c r="D53" s="90" t="s">
+        <v>228</v>
       </c>
       <c r="E53" s="89"/>
-      <c r="F53" s="90" t="s">
-        <v>228</v>
-      </c>
-      <c r="G53" s="89"/>
+      <c r="F53" s="89" t="s">
+        <v>268</v>
+      </c>
+      <c r="G53" s="89" t="s">
+        <v>102</v>
+      </c>
       <c r="H53" s="89" t="s">
-        <v>268</v>
-      </c>
-      <c r="I53" s="89" t="s">
-        <v>102</v>
-      </c>
-      <c r="J53" s="89" t="s">
         <v>339</v>
       </c>
-      <c r="K53" s="39" t="s">
+      <c r="I53" s="39" t="s">
         <v>14</v>
       </c>
     </row>
@@ -9445,8 +9412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B190E994-F93E-614B-8348-06136D69F1B4}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView zoomScale="131" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
cleaned up pre-processing scripts and add graphs scripts for each measure
</commit_message>
<xml_diff>
--- a/notes/conditions.xlsx
+++ b/notes/conditions.xlsx
@@ -1,29 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/momo/Dropbox/projects/connectives-qud/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2370B3-A45A-AF45-9632-A96CF471C8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF54ECF-31C3-FE4A-B676-9AD70C86A5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="820" windowWidth="35840" windowHeight="15860" activeTab="1" xr2:uid="{3AB9929D-0A0B-1747-A8A7-16F45675C35B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20240" activeTab="1" xr2:uid="{3AB9929D-0A0B-1747-A8A7-16F45675C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="overall" sheetId="9" r:id="rId1"/>
     <sheet name="new good test items" sheetId="11" r:id="rId2"/>
-    <sheet name="newSpecific-Working" sheetId="13" r:id="rId3"/>
-    <sheet name="critical_specificQUD" sheetId="14" r:id="rId4"/>
-    <sheet name="training" sheetId="6" r:id="rId5"/>
-    <sheet name="fillers" sheetId="5" r:id="rId6"/>
-    <sheet name="fillers_noQUD" sheetId="16" r:id="rId7"/>
-    <sheet name="training_noQUD" sheetId="17" r:id="rId8"/>
-    <sheet name="critical_generalQUD" sheetId="7" r:id="rId9"/>
-    <sheet name="critical_NoQUD" sheetId="8" r:id="rId10"/>
-    <sheet name="old_specificQUD" sheetId="4" r:id="rId11"/>
+    <sheet name="newcoding" sheetId="19" r:id="rId3"/>
+    <sheet name="newSpecific-Working" sheetId="13" r:id="rId4"/>
+    <sheet name="critical_specificQUD" sheetId="14" r:id="rId5"/>
+    <sheet name="training" sheetId="6" r:id="rId6"/>
+    <sheet name="fillers" sheetId="5" r:id="rId7"/>
+    <sheet name="fillers_noQUD" sheetId="16" r:id="rId8"/>
+    <sheet name="training_noQUD" sheetId="17" r:id="rId9"/>
+    <sheet name="critical_generalQUD" sheetId="7" r:id="rId10"/>
+    <sheet name="Feuil1" sheetId="18" r:id="rId11"/>
+    <sheet name="critical_NoQUD" sheetId="8" r:id="rId12"/>
+    <sheet name="old_specificQUD" sheetId="4" r:id="rId13"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3072" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3380" uniqueCount="392">
   <si>
     <t>QUD</t>
   </si>
@@ -1178,13 +1180,55 @@
   </si>
   <si>
     <t>aff</t>
+  </si>
+  <si>
+    <t>Ans-Mention</t>
+  </si>
+  <si>
+    <t>green and yellow items should all be the same for noQUD and General QUD because they mention a letter that's actually in the set of letters shown</t>
+  </si>
+  <si>
+    <t>notMention</t>
+  </si>
+  <si>
+    <t>prediction: 'but' takes longer when FC is Mention</t>
+  </si>
+  <si>
+    <t>Mention</t>
+  </si>
+  <si>
+    <t>Negation</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>AnsQUDRelevant</t>
+  </si>
+  <si>
+    <t>AnsConj1</t>
+  </si>
+  <si>
+    <t>QUDMention</t>
+  </si>
+  <si>
+    <t>AnsMention</t>
+  </si>
+  <si>
+    <t>yn</t>
+  </si>
+  <si>
+    <t>QUDType</t>
+  </si>
+  <si>
+    <t>Specific</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1207,8 +1251,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1267,6 +1324,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF9A8BFC"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1399,7 +1462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1506,6 +1569,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5090,6 +5165,1590 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468B3338-8DB1-0C41-9F65-FD8573AFE35E}">
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView zoomScale="132" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="K1" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+    </row>
+    <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="C11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="38">
+        <v>1</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14" s="39" t="s">
+        <v>213</v>
+      </c>
+      <c r="K14" s="40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="41">
+        <v>2</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" t="s">
+        <v>134</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G15" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="I15" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="J15" s="42" t="s">
+        <v>213</v>
+      </c>
+      <c r="K15" s="43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="44">
+        <v>3</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="45" t="s">
+        <v>166</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G16" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="J16" s="45" t="s">
+        <v>215</v>
+      </c>
+      <c r="K16" s="46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="41">
+        <v>4</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="I17" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="J17" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="K17" s="43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="44">
+        <v>5</v>
+      </c>
+      <c r="B18" s="45" t="s">
+        <v>254</v>
+      </c>
+      <c r="C18" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G18" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="I18" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="J18" s="45" t="s">
+        <v>214</v>
+      </c>
+      <c r="K18" s="46" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="41">
+        <v>6</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="C19" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G19" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="I19" s="42" t="s">
+        <v>259</v>
+      </c>
+      <c r="J19" s="42" t="s">
+        <v>214</v>
+      </c>
+      <c r="K19" s="43" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="38">
+        <v>7</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" t="s">
+        <v>135</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G20" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="I20" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="J20" s="39" t="s">
+        <v>214</v>
+      </c>
+      <c r="K20" s="40" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="38">
+        <v>8</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" t="s">
+        <v>134</v>
+      </c>
+      <c r="E21" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G21" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="I21" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="J21" s="39" t="s">
+        <v>214</v>
+      </c>
+      <c r="K21" s="40" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="44">
+        <v>9</v>
+      </c>
+      <c r="B22" s="45" t="s">
+        <v>260</v>
+      </c>
+      <c r="C22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D22" t="s">
+        <v>135</v>
+      </c>
+      <c r="E22" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G22" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="I22" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="J22" s="45" t="s">
+        <v>215</v>
+      </c>
+      <c r="K22" s="46" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="38">
+        <v>10</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>264</v>
+      </c>
+      <c r="C23" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G23" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" s="39" t="s">
+        <v>263</v>
+      </c>
+      <c r="I23" s="39" t="s">
+        <v>265</v>
+      </c>
+      <c r="J23" s="39" t="s">
+        <v>215</v>
+      </c>
+      <c r="K23" s="40" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="44">
+        <v>11</v>
+      </c>
+      <c r="B24" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="C24" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" t="s">
+        <v>135</v>
+      </c>
+      <c r="E24" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G24" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="I24" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="J24" s="45" t="s">
+        <v>213</v>
+      </c>
+      <c r="K24" s="46" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="41">
+        <v>12</v>
+      </c>
+      <c r="B25" s="42" t="s">
+        <v>269</v>
+      </c>
+      <c r="C25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D25" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G25" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="I25" s="42" t="s">
+        <v>271</v>
+      </c>
+      <c r="J25" s="42" t="s">
+        <v>213</v>
+      </c>
+      <c r="K25" s="43" t="s">
+        <v>245</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4B70A3-3ED8-EE4E-8063-2B680E725879}">
+  <dimension ref="A1:H29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="84">
+        <v>3</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="85" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" s="85" t="s">
+        <v>345</v>
+      </c>
+      <c r="E4" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="85" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="86">
+        <v>4</v>
+      </c>
+      <c r="B5" s="87" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="88" t="s">
+        <v>166</v>
+      </c>
+      <c r="D5" s="89" t="s">
+        <v>345</v>
+      </c>
+      <c r="E5" s="88" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="87" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="87" t="s">
+        <v>234</v>
+      </c>
+      <c r="H5" s="88" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="84">
+        <v>5</v>
+      </c>
+      <c r="B6" s="85" t="s">
+        <v>236</v>
+      </c>
+      <c r="C6" s="85" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" s="85" t="s">
+        <v>345</v>
+      </c>
+      <c r="E6" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="85" t="s">
+        <v>237</v>
+      </c>
+      <c r="G6" s="85" t="s">
+        <v>172</v>
+      </c>
+      <c r="H6" s="85" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="86">
+        <v>6</v>
+      </c>
+      <c r="B7" s="88" t="s">
+        <v>238</v>
+      </c>
+      <c r="C7" s="88" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" s="89" t="s">
+        <v>345</v>
+      </c>
+      <c r="E7" s="88" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="88" t="s">
+        <v>241</v>
+      </c>
+      <c r="G7" s="88" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="88" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="84">
+        <v>9</v>
+      </c>
+      <c r="B10" s="85" t="s">
+        <v>242</v>
+      </c>
+      <c r="C10" s="85" t="s">
+        <v>168</v>
+      </c>
+      <c r="D10" s="85" t="s">
+        <v>345</v>
+      </c>
+      <c r="E10" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="85" t="s">
+        <v>244</v>
+      </c>
+      <c r="G10" s="85" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" s="85" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="90">
+        <v>10</v>
+      </c>
+      <c r="B11" s="87" t="s">
+        <v>246</v>
+      </c>
+      <c r="C11" s="87" t="s">
+        <v>168</v>
+      </c>
+      <c r="D11" s="89" t="s">
+        <v>345</v>
+      </c>
+      <c r="E11" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="87" t="s">
+        <v>248</v>
+      </c>
+      <c r="G11" s="87" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="87" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="84">
+        <v>11</v>
+      </c>
+      <c r="B12" s="85" t="s">
+        <v>249</v>
+      </c>
+      <c r="C12" s="85" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="85" t="s">
+        <v>345</v>
+      </c>
+      <c r="E12" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="85" t="s">
+        <v>220</v>
+      </c>
+      <c r="G12" s="85" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="85" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="86">
+        <v>12</v>
+      </c>
+      <c r="B13" s="88" t="s">
+        <v>251</v>
+      </c>
+      <c r="C13" s="88" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="89" t="s">
+        <v>345</v>
+      </c>
+      <c r="E13" s="88" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="88" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="88" t="s">
+        <v>253</v>
+      </c>
+      <c r="H13" s="88" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="68"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="38">
+        <v>1</v>
+      </c>
+      <c r="B15" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="39" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="41">
+        <v>2</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="42" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="84">
+        <v>3</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="85" t="s">
+        <v>166</v>
+      </c>
+      <c r="D17" s="85" t="s">
+        <v>345</v>
+      </c>
+      <c r="E17" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H17" s="85" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="86">
+        <v>4</v>
+      </c>
+      <c r="B18" s="88" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="88" t="s">
+        <v>166</v>
+      </c>
+      <c r="D18" s="89" t="s">
+        <v>345</v>
+      </c>
+      <c r="E18" s="88" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="88" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18" s="88" t="s">
+        <v>88</v>
+      </c>
+      <c r="H18" s="88" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="84">
+        <v>5</v>
+      </c>
+      <c r="B19" s="85" t="s">
+        <v>254</v>
+      </c>
+      <c r="C19" s="85" t="s">
+        <v>168</v>
+      </c>
+      <c r="D19" s="85" t="s">
+        <v>345</v>
+      </c>
+      <c r="E19" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="85" t="s">
+        <v>195</v>
+      </c>
+      <c r="G19" s="85" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" s="85" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="86">
+        <v>6</v>
+      </c>
+      <c r="B20" s="88" t="s">
+        <v>256</v>
+      </c>
+      <c r="C20" s="88" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" s="89" t="s">
+        <v>345</v>
+      </c>
+      <c r="E20" s="88" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="88" t="s">
+        <v>258</v>
+      </c>
+      <c r="G20" s="88" t="s">
+        <v>259</v>
+      </c>
+      <c r="H20" s="88" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="38">
+        <v>7</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="E21" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" s="39" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="38">
+        <v>8</v>
+      </c>
+      <c r="B22" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="H22" s="39" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="84">
+        <v>9</v>
+      </c>
+      <c r="B23" s="85" t="s">
+        <v>260</v>
+      </c>
+      <c r="C23" s="85" t="s">
+        <v>168</v>
+      </c>
+      <c r="D23" s="85" t="s">
+        <v>345</v>
+      </c>
+      <c r="E23" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="85" t="s">
+        <v>189</v>
+      </c>
+      <c r="G23" s="85" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="85" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="90">
+        <v>10</v>
+      </c>
+      <c r="B24" s="87" t="s">
+        <v>264</v>
+      </c>
+      <c r="C24" s="87" t="s">
+        <v>168</v>
+      </c>
+      <c r="D24" s="89" t="s">
+        <v>345</v>
+      </c>
+      <c r="E24" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="87" t="s">
+        <v>263</v>
+      </c>
+      <c r="G24" s="87" t="s">
+        <v>265</v>
+      </c>
+      <c r="H24" s="87" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="84">
+        <v>11</v>
+      </c>
+      <c r="B25" s="85" t="s">
+        <v>266</v>
+      </c>
+      <c r="C25" s="85" t="s">
+        <v>167</v>
+      </c>
+      <c r="D25" s="85" t="s">
+        <v>345</v>
+      </c>
+      <c r="E25" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="85" t="s">
+        <v>267</v>
+      </c>
+      <c r="G25" s="85" t="s">
+        <v>52</v>
+      </c>
+      <c r="H25" s="85" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="86">
+        <v>12</v>
+      </c>
+      <c r="B26" s="88" t="s">
+        <v>269</v>
+      </c>
+      <c r="C26" s="88" t="s">
+        <v>167</v>
+      </c>
+      <c r="D26" s="89" t="s">
+        <v>345</v>
+      </c>
+      <c r="E26" s="88" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="88" t="s">
+        <v>270</v>
+      </c>
+      <c r="G26" s="88" t="s">
+        <v>271</v>
+      </c>
+      <c r="H26" s="88" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D29" s="15" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F873FAA-6FD8-C34F-8D74-6DAC069514F6}">
   <dimension ref="A1:M25"/>
   <sheetViews>
@@ -5984,7 +7643,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC7F87A-D3A0-7643-A0A1-BADC795412EC}">
   <dimension ref="A1:P19"/>
   <sheetViews>
@@ -6774,7 +8433,7 @@
   <dimension ref="A1:X58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6857,7 +8516,9 @@
       <c r="J2" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="K2" s="13"/>
+      <c r="K2" s="11" t="s">
+        <v>380</v>
+      </c>
       <c r="L2" s="13"/>
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
@@ -6901,7 +8562,9 @@
       <c r="J3" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="K3" s="13"/>
+      <c r="K3" s="11" t="s">
+        <v>380</v>
+      </c>
       <c r="L3" s="13"/>
       <c r="M3" s="13"/>
       <c r="N3" s="13"/>
@@ -6943,7 +8606,9 @@
         <v>5</v>
       </c>
       <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
+      <c r="K4" s="11" t="s">
+        <v>378</v>
+      </c>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
@@ -6985,7 +8650,9 @@
         <v>5</v>
       </c>
       <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
+      <c r="K5" s="11" t="s">
+        <v>378</v>
+      </c>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
@@ -7027,7 +8694,9 @@
         <v>219</v>
       </c>
       <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
+      <c r="K6" s="11" t="s">
+        <v>378</v>
+      </c>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
@@ -7069,7 +8738,9 @@
         <v>219</v>
       </c>
       <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
+      <c r="K7" s="11" t="s">
+        <v>378</v>
+      </c>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
@@ -7113,7 +8784,9 @@
       <c r="J8" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="K8" s="13"/>
+      <c r="K8" s="11" t="s">
+        <v>380</v>
+      </c>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
@@ -7157,7 +8830,9 @@
       <c r="J9" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="K9" s="13"/>
+      <c r="K9" s="11" t="s">
+        <v>380</v>
+      </c>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
@@ -7199,7 +8874,9 @@
         <v>245</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="13"/>
+      <c r="K10" s="11" t="s">
+        <v>378</v>
+      </c>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
@@ -7241,7 +8918,9 @@
         <v>245</v>
       </c>
       <c r="J11" s="1"/>
-      <c r="K11" s="13"/>
+      <c r="K11" s="11" t="s">
+        <v>378</v>
+      </c>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
@@ -7282,6 +8961,9 @@
       <c r="I12" s="5" t="s">
         <v>245</v>
       </c>
+      <c r="K12" s="11" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
@@ -7312,7 +8994,9 @@
         <v>245</v>
       </c>
       <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
+      <c r="K13" s="11" t="s">
+        <v>378</v>
+      </c>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
       <c r="N13" s="13"/>
@@ -7404,7 +9088,9 @@
         <v>366</v>
       </c>
       <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
+      <c r="I16" s="11" t="s">
+        <v>381</v>
+      </c>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
@@ -8383,6 +10069,445 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B3E625-C32F-394F-B0FD-4D2293454ECA}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView zoomScale="162" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="21.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="13.5" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="92" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="92" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="92" t="s">
+        <v>386</v>
+      </c>
+      <c r="E1" s="92" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="92" t="s">
+        <v>390</v>
+      </c>
+      <c r="G1" s="92" t="s">
+        <v>385</v>
+      </c>
+      <c r="H1" s="92" t="s">
+        <v>383</v>
+      </c>
+      <c r="I1" s="93" t="s">
+        <v>388</v>
+      </c>
+      <c r="J1" s="92" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="91">
+        <v>1</v>
+      </c>
+      <c r="B2" s="91" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="91" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" s="91" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="91" t="s">
+        <v>391</v>
+      </c>
+      <c r="G2" s="91" t="s">
+        <v>384</v>
+      </c>
+      <c r="H2" s="91" t="s">
+        <v>317</v>
+      </c>
+      <c r="I2" s="91" t="s">
+        <v>380</v>
+      </c>
+      <c r="J2" s="91" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="91">
+        <v>2</v>
+      </c>
+      <c r="B3" s="91" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="91" t="s">
+        <v>216</v>
+      </c>
+      <c r="D3" s="91" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="91" t="s">
+        <v>391</v>
+      </c>
+      <c r="G3" s="91" t="s">
+        <v>384</v>
+      </c>
+      <c r="H3" s="91" t="s">
+        <v>317</v>
+      </c>
+      <c r="I3" s="91" t="s">
+        <v>380</v>
+      </c>
+      <c r="J3" s="91" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="91">
+        <v>3</v>
+      </c>
+      <c r="B4" s="91" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="91" t="s">
+        <v>216</v>
+      </c>
+      <c r="D4" s="91" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="91" t="s">
+        <v>391</v>
+      </c>
+      <c r="G4" s="91" t="s">
+        <v>317</v>
+      </c>
+      <c r="H4" s="91" t="s">
+        <v>384</v>
+      </c>
+      <c r="I4" s="91" t="s">
+        <v>382</v>
+      </c>
+      <c r="J4" s="91" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="91">
+        <v>4</v>
+      </c>
+      <c r="B5" s="91" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="91" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" s="91" t="s">
+        <v>190</v>
+      </c>
+      <c r="E5" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="91" t="s">
+        <v>391</v>
+      </c>
+      <c r="G5" s="91" t="s">
+        <v>317</v>
+      </c>
+      <c r="H5" s="91" t="s">
+        <v>384</v>
+      </c>
+      <c r="I5" s="91" t="s">
+        <v>382</v>
+      </c>
+      <c r="J5" s="91" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="91">
+        <v>5</v>
+      </c>
+      <c r="B6" s="91" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="91" t="s">
+        <v>217</v>
+      </c>
+      <c r="D6" s="91" t="s">
+        <v>189</v>
+      </c>
+      <c r="E6" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="91" t="s">
+        <v>391</v>
+      </c>
+      <c r="G6" s="91" t="s">
+        <v>317</v>
+      </c>
+      <c r="H6" s="91" t="s">
+        <v>384</v>
+      </c>
+      <c r="I6" s="91" t="s">
+        <v>382</v>
+      </c>
+      <c r="J6" s="91" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="91">
+        <v>6</v>
+      </c>
+      <c r="B7" s="91" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="91" t="s">
+        <v>217</v>
+      </c>
+      <c r="D7" s="91" t="s">
+        <v>190</v>
+      </c>
+      <c r="E7" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="91" t="s">
+        <v>391</v>
+      </c>
+      <c r="G7" s="91" t="s">
+        <v>317</v>
+      </c>
+      <c r="H7" s="91" t="s">
+        <v>384</v>
+      </c>
+      <c r="I7" s="91" t="s">
+        <v>382</v>
+      </c>
+      <c r="J7" s="91" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="91">
+        <v>7</v>
+      </c>
+      <c r="B8" s="91" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="91" t="s">
+        <v>218</v>
+      </c>
+      <c r="D8" s="91" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="91" t="s">
+        <v>391</v>
+      </c>
+      <c r="G8" s="91" t="s">
+        <v>317</v>
+      </c>
+      <c r="H8" s="91" t="s">
+        <v>317</v>
+      </c>
+      <c r="I8" s="91" t="s">
+        <v>380</v>
+      </c>
+      <c r="J8" s="91" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="91">
+        <v>8</v>
+      </c>
+      <c r="B9" s="91" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="91" t="s">
+        <v>218</v>
+      </c>
+      <c r="D9" s="91" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="91" t="s">
+        <v>391</v>
+      </c>
+      <c r="G9" s="91" t="s">
+        <v>317</v>
+      </c>
+      <c r="H9" s="91" t="s">
+        <v>317</v>
+      </c>
+      <c r="I9" s="91" t="s">
+        <v>380</v>
+      </c>
+      <c r="J9" s="91" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="91">
+        <v>9</v>
+      </c>
+      <c r="B10" s="91" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" s="91" t="s">
+        <v>217</v>
+      </c>
+      <c r="D10" s="91" t="s">
+        <v>189</v>
+      </c>
+      <c r="E10" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="91" t="s">
+        <v>391</v>
+      </c>
+      <c r="G10" s="91" t="s">
+        <v>317</v>
+      </c>
+      <c r="H10" s="91" t="s">
+        <v>384</v>
+      </c>
+      <c r="I10" s="91" t="s">
+        <v>382</v>
+      </c>
+      <c r="J10" s="91" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="91">
+        <v>10</v>
+      </c>
+      <c r="B11" s="91" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="91" t="s">
+        <v>217</v>
+      </c>
+      <c r="D11" s="91" t="s">
+        <v>190</v>
+      </c>
+      <c r="E11" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="91" t="s">
+        <v>391</v>
+      </c>
+      <c r="G11" s="91" t="s">
+        <v>317</v>
+      </c>
+      <c r="H11" s="91" t="s">
+        <v>384</v>
+      </c>
+      <c r="I11" s="91" t="s">
+        <v>382</v>
+      </c>
+      <c r="J11" s="91" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="91">
+        <v>11</v>
+      </c>
+      <c r="B12" s="91" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="91" t="s">
+        <v>218</v>
+      </c>
+      <c r="D12" s="91" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="91" t="s">
+        <v>391</v>
+      </c>
+      <c r="G12" s="91" t="s">
+        <v>384</v>
+      </c>
+      <c r="H12" s="91" t="s">
+        <v>384</v>
+      </c>
+      <c r="I12" s="91" t="s">
+        <v>382</v>
+      </c>
+      <c r="J12" s="91" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="91">
+        <v>12</v>
+      </c>
+      <c r="B13" s="91" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="91" t="s">
+        <v>218</v>
+      </c>
+      <c r="D13" s="91" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="91" t="s">
+        <v>391</v>
+      </c>
+      <c r="G13" s="91" t="s">
+        <v>384</v>
+      </c>
+      <c r="H13" s="91" t="s">
+        <v>384</v>
+      </c>
+      <c r="I13" s="91" t="s">
+        <v>382</v>
+      </c>
+      <c r="J13" s="91" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666AB419-CDE0-1C4A-A8E9-4783315D873D}">
   <dimension ref="A1:X39"/>
   <sheetViews>
@@ -10253,16 +12378,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0226BAE4-5B3C-9C46-8158-4454A2BE036C}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="167" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="6" max="6" width="23.83203125" customWidth="1"/>
     <col min="8" max="8" width="23" customWidth="1"/>
     <col min="9" max="9" width="17.83203125" customWidth="1"/>
   </cols>
@@ -11147,7 +13273,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4DBC4F9-E0E7-324A-AE5A-00B4893BD830}">
   <dimension ref="A1:P5"/>
   <sheetViews>
@@ -11335,12 +13461,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B190E994-F93E-614B-8348-06136D69F1B4}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="131" workbookViewId="0">
-      <selection activeCell="M19" sqref="A1:XFD1048576"/>
+    <sheetView zoomScale="131" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12233,7 +14359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5530880F-CA27-7B4B-9D22-D13AC1FFEBD8}">
   <dimension ref="A1:O32"/>
   <sheetViews>
@@ -13155,7 +15281,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{644A2E13-A585-1544-8804-CED5AB2073E6}">
   <dimension ref="A1:L5"/>
   <sheetViews>
@@ -13334,901 +15460,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468B3338-8DB1-0C41-9F65-FD8573AFE35E}">
-  <dimension ref="A1:N25"/>
-  <sheetViews>
-    <sheetView zoomScale="132" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="6" max="6" width="26.6640625" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="13"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>231</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J1" s="33" t="s">
-        <v>230</v>
-      </c>
-      <c r="K1" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-    </row>
-    <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" t="s">
-        <v>134</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="C6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="C7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D7" t="s">
-        <v>134</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
-        <v>7</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
-        <v>8</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D9" t="s">
-        <v>134</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="C10" t="s">
-        <v>134</v>
-      </c>
-      <c r="D10" t="s">
-        <v>135</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>10</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="C11" t="s">
-        <v>135</v>
-      </c>
-      <c r="D11" t="s">
-        <v>134</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="C12" t="s">
-        <v>134</v>
-      </c>
-      <c r="D12" t="s">
-        <v>135</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>12</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="C13" t="s">
-        <v>135</v>
-      </c>
-      <c r="D13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38">
-        <v>1</v>
-      </c>
-      <c r="B14" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" t="s">
-        <v>134</v>
-      </c>
-      <c r="D14" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G14" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="I14" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="J14" s="39" t="s">
-        <v>213</v>
-      </c>
-      <c r="K14" s="40" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41">
-        <v>2</v>
-      </c>
-      <c r="B15" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" t="s">
-        <v>135</v>
-      </c>
-      <c r="D15" t="s">
-        <v>134</v>
-      </c>
-      <c r="E15" s="42" t="s">
-        <v>166</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G15" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="I15" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="J15" s="42" t="s">
-        <v>213</v>
-      </c>
-      <c r="K15" s="43" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="44">
-        <v>3</v>
-      </c>
-      <c r="B16" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" t="s">
-        <v>134</v>
-      </c>
-      <c r="D16" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" s="45" t="s">
-        <v>166</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G16" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="H16" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="J16" s="45" t="s">
-        <v>215</v>
-      </c>
-      <c r="K16" s="46" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="41">
-        <v>4</v>
-      </c>
-      <c r="B17" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" t="s">
-        <v>135</v>
-      </c>
-      <c r="D17" t="s">
-        <v>134</v>
-      </c>
-      <c r="E17" s="42" t="s">
-        <v>166</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G17" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="I17" s="42" t="s">
-        <v>88</v>
-      </c>
-      <c r="J17" s="42" t="s">
-        <v>215</v>
-      </c>
-      <c r="K17" s="43" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="44">
-        <v>5</v>
-      </c>
-      <c r="B18" s="45" t="s">
-        <v>254</v>
-      </c>
-      <c r="C18" t="s">
-        <v>134</v>
-      </c>
-      <c r="D18" t="s">
-        <v>135</v>
-      </c>
-      <c r="E18" s="45" t="s">
-        <v>168</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G18" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="45" t="s">
-        <v>195</v>
-      </c>
-      <c r="I18" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="J18" s="45" t="s">
-        <v>214</v>
-      </c>
-      <c r="K18" s="46" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41">
-        <v>6</v>
-      </c>
-      <c r="B19" s="42" t="s">
-        <v>256</v>
-      </c>
-      <c r="C19" t="s">
-        <v>135</v>
-      </c>
-      <c r="D19" t="s">
-        <v>134</v>
-      </c>
-      <c r="E19" s="42" t="s">
-        <v>168</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G19" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="42" t="s">
-        <v>258</v>
-      </c>
-      <c r="I19" s="42" t="s">
-        <v>259</v>
-      </c>
-      <c r="J19" s="42" t="s">
-        <v>214</v>
-      </c>
-      <c r="K19" s="43" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="38">
-        <v>7</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" t="s">
-        <v>134</v>
-      </c>
-      <c r="D20" t="s">
-        <v>135</v>
-      </c>
-      <c r="E20" s="39" t="s">
-        <v>167</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G20" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="H20" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="I20" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="J20" s="39" t="s">
-        <v>214</v>
-      </c>
-      <c r="K20" s="40" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="38">
-        <v>8</v>
-      </c>
-      <c r="B21" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" t="s">
-        <v>135</v>
-      </c>
-      <c r="D21" t="s">
-        <v>134</v>
-      </c>
-      <c r="E21" s="39" t="s">
-        <v>167</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G21" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="I21" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="J21" s="39" t="s">
-        <v>214</v>
-      </c>
-      <c r="K21" s="40" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="44">
-        <v>9</v>
-      </c>
-      <c r="B22" s="45" t="s">
-        <v>260</v>
-      </c>
-      <c r="C22" t="s">
-        <v>134</v>
-      </c>
-      <c r="D22" t="s">
-        <v>135</v>
-      </c>
-      <c r="E22" s="45" t="s">
-        <v>168</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G22" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="H22" s="45" t="s">
-        <v>189</v>
-      </c>
-      <c r="I22" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="J22" s="45" t="s">
-        <v>215</v>
-      </c>
-      <c r="K22" s="46" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="38">
-        <v>10</v>
-      </c>
-      <c r="B23" s="39" t="s">
-        <v>264</v>
-      </c>
-      <c r="C23" t="s">
-        <v>135</v>
-      </c>
-      <c r="D23" t="s">
-        <v>134</v>
-      </c>
-      <c r="E23" s="39" t="s">
-        <v>168</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G23" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="H23" s="39" t="s">
-        <v>263</v>
-      </c>
-      <c r="I23" s="39" t="s">
-        <v>265</v>
-      </c>
-      <c r="J23" s="39" t="s">
-        <v>215</v>
-      </c>
-      <c r="K23" s="40" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="44">
-        <v>11</v>
-      </c>
-      <c r="B24" s="45" t="s">
-        <v>266</v>
-      </c>
-      <c r="C24" t="s">
-        <v>134</v>
-      </c>
-      <c r="D24" t="s">
-        <v>135</v>
-      </c>
-      <c r="E24" s="45" t="s">
-        <v>167</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G24" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="H24" s="45" t="s">
-        <v>267</v>
-      </c>
-      <c r="I24" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="J24" s="45" t="s">
-        <v>213</v>
-      </c>
-      <c r="K24" s="46" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="41">
-        <v>12</v>
-      </c>
-      <c r="B25" s="42" t="s">
-        <v>269</v>
-      </c>
-      <c r="C25" t="s">
-        <v>135</v>
-      </c>
-      <c r="D25" t="s">
-        <v>134</v>
-      </c>
-      <c r="E25" s="42" t="s">
-        <v>167</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="G25" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="H25" s="42" t="s">
-        <v>270</v>
-      </c>
-      <c r="I25" s="42" t="s">
-        <v>271</v>
-      </c>
-      <c r="J25" s="42" t="s">
-        <v>213</v>
-      </c>
-      <c r="K25" s="43" t="s">
-        <v>245</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>